<commit_message>
created GUI for data loader
</commit_message>
<xml_diff>
--- a/Database Test Plugin.xlsx
+++ b/Database Test Plugin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pum001f\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pum001f\Desktop\DatabaseInserter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D844A6-AFA4-40FB-A264-84AFB60ABCCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76E2706-B39F-4872-BB96-2F4075B6A29C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{9959ACE3-6C34-4D54-AD38-4738E412C3D3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="133">
   <si>
     <t>Orchestrator Number</t>
   </si>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76BBFAB6-1D74-47B5-9041-32482670E62E}">
   <dimension ref="A1:BY4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="73" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1406,7 +1406,9 @@
       </c>
       <c r="AL2" s="15"/>
       <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
+      <c r="AN2" s="15" t="s">
+        <v>68</v>
+      </c>
       <c r="AO2" s="14" t="s">
         <v>50</v>
       </c>

</xml_diff>